<commit_message>
updated project details excel
</commit_message>
<xml_diff>
--- a/doc/Projektdetails_WS24_Gruppe_2.xlsx
+++ b/doc/Projektdetails_WS24_Gruppe_2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilijakostic/Documents/FH/Sem3/Objektorientierte_Dienstentwicklung/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilijakostic/Desktop/BlackJack/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB61B6EE-11E7-4144-BF7D-42B94B519880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA1C7F1-D56C-BF4B-9965-6C5F71FD70F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="155">
   <si>
     <t>Informationen</t>
   </si>
@@ -897,15 +897,6 @@
   </si>
   <si>
     <t>Plannung und Organisation</t>
-  </si>
-  <si>
-    <t>Must have feature Implementierung</t>
-  </si>
-  <si>
-    <t>5h</t>
-  </si>
-  <si>
-    <t>noch nicht gemerged</t>
   </si>
   <si>
     <t>Aufteilung der Themen
@@ -8809,7 +8800,7 @@
   <dimension ref="B2:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -8883,7 +8874,7 @@
         <v>153</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>146</v>
@@ -8909,47 +8900,23 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="42">
-      <c r="B7" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="42">
-      <c r="B8" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="42">
-      <c r="B9" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>156</v>
-      </c>
+    <row r="7" spans="2:7" ht="13">
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+    </row>
+    <row r="8" spans="2:7" ht="13">
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+    </row>
+    <row r="9" spans="2:7" ht="13">
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>